<commit_message>
generate translations on server
</commit_message>
<xml_diff>
--- a/server/translations.xlsx
+++ b/server/translations.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>ru</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>not found</t>
+  </si>
+  <si>
+    <t>_name</t>
   </si>
 </sst>
 </file>
@@ -410,9 +410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -424,72 +422,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>